<commit_message>
update hok and persday for hp
</commit_message>
<xml_diff>
--- a/shiny/data/template/raw data untuk crosscek pam baru.xlsx
+++ b/shiny/data/template/raw data untuk crosscek pam baru.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://icrafcifor-my.sharepoint.com/personal/d_bodro_cifor-icraf_org/Documents/dw/project R/theme 2/lusita/shiny/data/template/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{C9953028-729E-4230-BDED-2387E9D6C9CC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="32" documentId="8_{C9953028-729E-4230-BDED-2387E9D6C9CC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{F67D9DDD-D9DA-41CF-80F6-09A90E90B319}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="24240" windowHeight="13020" xr2:uid="{434F79F2-1D89-4230-B38A-FBCE8A0F0489}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{434F79F2-1D89-4230-B38A-FBCE8A0F0489}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="146" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="156" uniqueCount="57">
   <si>
     <t>Urea</t>
   </si>
@@ -174,13 +174,50 @@
   </si>
   <si>
     <t>Rp/HOK</t>
+  </si>
+  <si>
+    <t>Asumsi Mikro Ekonomi</t>
+  </si>
+  <si>
+    <t>Discount rate</t>
+  </si>
+  <si>
+    <t>%</t>
+  </si>
+  <si>
+    <t>Upah buruh</t>
+  </si>
+  <si>
+    <t>Nilai tukar rupiah</t>
+  </si>
+  <si>
+    <t>USD</t>
+  </si>
+  <si>
+    <t>tenaga kerja</t>
+  </si>
+  <si>
+    <t>kerja</t>
+  </si>
+  <si>
+    <t>"tenaga kerja|tk|kerja|tenaga"</t>
+  </si>
+  <si>
+    <t>HARUS LOWCASE</t>
+  </si>
+  <si>
+    <t>"hok|HOK"</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <numFmts count="2">
+    <numFmt numFmtId="164" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="165" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)"/>
+  </numFmts>
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -188,13 +225,57 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -206,17 +287,31 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
+      <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="3" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="3" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="3" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="3" applyFont="1" applyFill="1"/>
+    <xf numFmtId="10" fontId="5" fillId="3" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="165" fontId="5" fillId="3" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="4">
+    <cellStyle name="Comma" xfId="1" builtinId="3"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal 2" xfId="3" xr:uid="{94FF5CB3-CD83-489A-AC5F-66153427EC2F}"/>
+    <cellStyle name="Percent" xfId="2" builtinId="5"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -229,6 +324,10 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -528,15 +627,24 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6E76978D-30F8-4CCF-8060-75D8D0F1ED70}">
-  <dimension ref="A1:AG66"/>
+  <dimension ref="A1:AG75"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A53" workbookViewId="0">
-      <selection activeCell="H61" sqref="H61"/>
+    <sheetView tabSelected="1" topLeftCell="A64" workbookViewId="0">
+      <selection activeCell="B75" sqref="B75"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="31" customWidth="1"/>
+    <col min="2" max="2" width="31" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="8" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="4" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="21.7265625" bestFit="1" customWidth="1"/>
+    <col min="6" max="27" width="12" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="7.54296875" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:33" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>38</v>
       </c>
@@ -546,8 +654,49 @@
       <c r="C1">
         <v>2023</v>
       </c>
-    </row>
-    <row r="5" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="E1" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="F1" s="3"/>
+      <c r="G1" s="3"/>
+    </row>
+    <row r="2" spans="1:33" x14ac:dyDescent="0.35">
+      <c r="A2" s="8" t="s">
+        <v>55</v>
+      </c>
+      <c r="E2" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="F2" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="G2" s="6">
+        <v>7.0199999999999999E-2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:33" x14ac:dyDescent="0.35">
+      <c r="E3" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="F3" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="G3" s="7">
+        <v>100000</v>
+      </c>
+    </row>
+    <row r="4" spans="1:33" x14ac:dyDescent="0.35">
+      <c r="E4" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="F4" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="G4" s="7">
+        <v>14775</v>
+      </c>
+    </row>
+    <row r="5" spans="1:33" x14ac:dyDescent="0.35">
       <c r="A5" s="1" t="s">
         <v>32</v>
       </c>
@@ -638,7 +787,7 @@
       <c r="AF5" s="1"/>
       <c r="AG5" s="1"/>
     </row>
-    <row r="6" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:33" x14ac:dyDescent="0.35">
       <c r="A6" s="1" t="s">
         <v>32</v>
       </c>
@@ -729,7 +878,7 @@
       <c r="AF6" s="1"/>
       <c r="AG6" s="1"/>
     </row>
-    <row r="7" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:33" x14ac:dyDescent="0.35">
       <c r="A7" s="1" t="s">
         <v>32</v>
       </c>
@@ -820,7 +969,7 @@
       <c r="AF7" s="1"/>
       <c r="AG7" s="1"/>
     </row>
-    <row r="8" spans="1:33" ht="30" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:33" x14ac:dyDescent="0.35">
       <c r="A8" s="1" t="s">
         <v>32</v>
       </c>
@@ -911,7 +1060,7 @@
       <c r="AF8" s="1"/>
       <c r="AG8" s="1"/>
     </row>
-    <row r="9" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:33" x14ac:dyDescent="0.35">
       <c r="A9" s="1" t="s">
         <v>32</v>
       </c>
@@ -1002,7 +1151,7 @@
       <c r="AF9" s="1"/>
       <c r="AG9" s="1"/>
     </row>
-    <row r="10" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:33" x14ac:dyDescent="0.35">
       <c r="A10" s="1" t="s">
         <v>32</v>
       </c>
@@ -1093,7 +1242,7 @@
       <c r="AF10" s="1"/>
       <c r="AG10" s="1"/>
     </row>
-    <row r="11" spans="1:33" ht="30" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:33" x14ac:dyDescent="0.35">
       <c r="A11" s="1" t="s">
         <v>32</v>
       </c>
@@ -1184,7 +1333,7 @@
       <c r="AF11" s="1"/>
       <c r="AG11" s="1"/>
     </row>
-    <row r="12" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:33" x14ac:dyDescent="0.35">
       <c r="A12" s="1" t="s">
         <v>33</v>
       </c>
@@ -1275,7 +1424,7 @@
       <c r="AF12" s="1"/>
       <c r="AG12" s="1"/>
     </row>
-    <row r="13" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:33" x14ac:dyDescent="0.35">
       <c r="A13" s="1" t="s">
         <v>33</v>
       </c>
@@ -1366,7 +1515,7 @@
       <c r="AF13" s="1"/>
       <c r="AG13" s="1"/>
     </row>
-    <row r="14" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:33" x14ac:dyDescent="0.35">
       <c r="A14" s="1" t="s">
         <v>33</v>
       </c>
@@ -1457,7 +1606,7 @@
       <c r="AF14" s="1"/>
       <c r="AG14" s="1"/>
     </row>
-    <row r="15" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:33" x14ac:dyDescent="0.35">
       <c r="A15" s="1" t="s">
         <v>33</v>
       </c>
@@ -1548,7 +1697,7 @@
       <c r="AF15" s="1"/>
       <c r="AG15" s="1"/>
     </row>
-    <row r="16" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:33" x14ac:dyDescent="0.35">
       <c r="A16" s="1" t="s">
         <v>33</v>
       </c>
@@ -1639,7 +1788,7 @@
       <c r="AF16" s="1"/>
       <c r="AG16" s="1"/>
     </row>
-    <row r="17" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:33" x14ac:dyDescent="0.35">
       <c r="A17" s="1" t="s">
         <v>33</v>
       </c>
@@ -1730,7 +1879,7 @@
       <c r="AF17" s="1"/>
       <c r="AG17" s="1"/>
     </row>
-    <row r="18" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:33" x14ac:dyDescent="0.35">
       <c r="A18" s="1" t="s">
         <v>33</v>
       </c>
@@ -1821,7 +1970,7 @@
       <c r="AF18" s="1"/>
       <c r="AG18" s="1"/>
     </row>
-    <row r="19" spans="1:33" ht="45" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:33" x14ac:dyDescent="0.35">
       <c r="A19" s="1" t="s">
         <v>33</v>
       </c>
@@ -1912,7 +2061,7 @@
       <c r="AF19" s="1"/>
       <c r="AG19" s="1"/>
     </row>
-    <row r="20" spans="1:33" ht="60" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:33" x14ac:dyDescent="0.35">
       <c r="A20" s="1" t="s">
         <v>33</v>
       </c>
@@ -2003,7 +2152,7 @@
       <c r="AF20" s="1"/>
       <c r="AG20" s="1"/>
     </row>
-    <row r="21" spans="1:33" ht="30" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:33" x14ac:dyDescent="0.35">
       <c r="A21" s="1" t="s">
         <v>33</v>
       </c>
@@ -2094,7 +2243,7 @@
       <c r="AF21" s="1"/>
       <c r="AG21" s="1"/>
     </row>
-    <row r="22" spans="1:33" ht="45" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:33" x14ac:dyDescent="0.35">
       <c r="A22" s="1" t="s">
         <v>33</v>
       </c>
@@ -2185,7 +2334,7 @@
       <c r="AF22" s="1"/>
       <c r="AG22" s="1"/>
     </row>
-    <row r="23" spans="1:33" ht="45" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:33" x14ac:dyDescent="0.35">
       <c r="A23" s="1" t="s">
         <v>33</v>
       </c>
@@ -2276,7 +2425,7 @@
       <c r="AF23" s="1"/>
       <c r="AG23" s="1"/>
     </row>
-    <row r="24" spans="1:33" ht="45" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:33" x14ac:dyDescent="0.35">
       <c r="A24" s="1" t="s">
         <v>34</v>
       </c>
@@ -2321,7 +2470,7 @@
       <c r="AF24" s="1"/>
       <c r="AG24" s="1"/>
     </row>
-    <row r="25" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:33" x14ac:dyDescent="0.35">
       <c r="A25" s="1" t="s">
         <v>35</v>
       </c>
@@ -2412,7 +2561,7 @@
       <c r="AF25" s="1"/>
       <c r="AG25" s="1"/>
     </row>
-    <row r="26" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:33" x14ac:dyDescent="0.35">
       <c r="A26" s="1" t="s">
         <v>35</v>
       </c>
@@ -2503,9 +2652,9 @@
       <c r="AF26" s="1"/>
       <c r="AG26" s="1"/>
     </row>
-    <row r="27" spans="1:33" ht="75" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:33" x14ac:dyDescent="0.35">
       <c r="A27" s="1" t="s">
-        <v>35</v>
+        <v>53</v>
       </c>
       <c r="B27" s="1" t="s">
         <v>26</v>
@@ -2594,9 +2743,9 @@
       <c r="AF27" s="1"/>
       <c r="AG27" s="1"/>
     </row>
-    <row r="28" spans="1:33" ht="45" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:33" x14ac:dyDescent="0.35">
       <c r="A28" s="1" t="s">
-        <v>35</v>
+        <v>53</v>
       </c>
       <c r="B28" s="1" t="s">
         <v>27</v>
@@ -2685,9 +2834,9 @@
       <c r="AF28" s="1"/>
       <c r="AG28" s="1"/>
     </row>
-    <row r="29" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:33" x14ac:dyDescent="0.35">
       <c r="A29" s="1" t="s">
-        <v>35</v>
+        <v>52</v>
       </c>
       <c r="B29" s="1" t="s">
         <v>28</v>
@@ -2776,9 +2925,9 @@
       <c r="AF29" s="1"/>
       <c r="AG29" s="1"/>
     </row>
-    <row r="30" spans="1:33" ht="30" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:33" x14ac:dyDescent="0.35">
       <c r="A30" s="1" t="s">
-        <v>35</v>
+        <v>52</v>
       </c>
       <c r="B30" s="1" t="s">
         <v>29</v>
@@ -2867,9 +3016,9 @@
       <c r="AF30" s="1"/>
       <c r="AG30" s="1"/>
     </row>
-    <row r="31" spans="1:33" ht="30" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:33" x14ac:dyDescent="0.35">
       <c r="A31" s="1" t="s">
-        <v>35</v>
+        <v>52</v>
       </c>
       <c r="B31" s="1" t="s">
         <v>30</v>
@@ -2958,9 +3107,9 @@
       <c r="AF31" s="1"/>
       <c r="AG31" s="1"/>
     </row>
-    <row r="32" spans="1:33" ht="30" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:33" x14ac:dyDescent="0.35">
       <c r="A32" s="1" t="s">
-        <v>35</v>
+        <v>52</v>
       </c>
       <c r="B32" s="1" t="s">
         <v>31</v>
@@ -3049,7 +3198,7 @@
       <c r="AF32" s="1"/>
       <c r="AG32" s="1"/>
     </row>
-    <row r="33" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:33" x14ac:dyDescent="0.35">
       <c r="A33" s="1"/>
       <c r="B33" s="1"/>
       <c r="C33" s="1"/>
@@ -3084,7 +3233,7 @@
       <c r="AF33" s="1"/>
       <c r="AG33" s="1"/>
     </row>
-    <row r="34" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:33" x14ac:dyDescent="0.35">
       <c r="A34" t="s">
         <v>36</v>
       </c>
@@ -3167,7 +3316,7 @@
         <v>18047.849207142859</v>
       </c>
     </row>
-    <row r="37" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:33" x14ac:dyDescent="0.35">
       <c r="A37" t="s">
         <v>0</v>
       </c>
@@ -3178,7 +3327,7 @@
         <v>9000</v>
       </c>
     </row>
-    <row r="38" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:33" x14ac:dyDescent="0.35">
       <c r="A38" t="s">
         <v>2</v>
       </c>
@@ -3189,7 +3338,7 @@
         <v>14000</v>
       </c>
     </row>
-    <row r="39" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:33" x14ac:dyDescent="0.35">
       <c r="A39" t="s">
         <v>3</v>
       </c>
@@ -3200,7 +3349,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="40" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:33" x14ac:dyDescent="0.35">
       <c r="A40" t="s">
         <v>4</v>
       </c>
@@ -3211,7 +3360,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="41" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:33" x14ac:dyDescent="0.35">
       <c r="A41" t="s">
         <v>5</v>
       </c>
@@ -3222,7 +3371,7 @@
         <v>90000</v>
       </c>
     </row>
-    <row r="42" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:33" x14ac:dyDescent="0.35">
       <c r="A42" t="s">
         <v>7</v>
       </c>
@@ -3233,7 +3382,7 @@
         <v>102000</v>
       </c>
     </row>
-    <row r="43" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:33" x14ac:dyDescent="0.35">
       <c r="A43" t="s">
         <v>9</v>
       </c>
@@ -3244,7 +3393,7 @@
         <v>95000</v>
       </c>
     </row>
-    <row r="44" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:33" x14ac:dyDescent="0.35">
       <c r="A44" t="s">
         <v>10</v>
       </c>
@@ -3255,7 +3404,7 @@
         <v>100000</v>
       </c>
     </row>
-    <row r="45" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:33" x14ac:dyDescent="0.35">
       <c r="A45" t="s">
         <v>12</v>
       </c>
@@ -3266,7 +3415,7 @@
         <v>38000</v>
       </c>
     </row>
-    <row r="46" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:33" x14ac:dyDescent="0.35">
       <c r="A46" t="s">
         <v>13</v>
       </c>
@@ -3277,7 +3426,7 @@
         <v>93000</v>
       </c>
     </row>
-    <row r="47" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:33" x14ac:dyDescent="0.35">
       <c r="A47" t="s">
         <v>14</v>
       </c>
@@ -3288,7 +3437,7 @@
         <v>585000</v>
       </c>
     </row>
-    <row r="48" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:33" x14ac:dyDescent="0.35">
       <c r="A48" t="s">
         <v>15</v>
       </c>
@@ -3299,7 +3448,7 @@
         <v>500000</v>
       </c>
     </row>
-    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A49" t="s">
         <v>16</v>
       </c>
@@ -3310,7 +3459,7 @@
         <v>460000</v>
       </c>
     </row>
-    <row r="50" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A50" t="s">
         <v>17</v>
       </c>
@@ -3321,7 +3470,7 @@
         <v>80000</v>
       </c>
     </row>
-    <row r="51" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A51" t="s">
         <v>18</v>
       </c>
@@ -3332,7 +3481,7 @@
         <v>5500000</v>
       </c>
     </row>
-    <row r="52" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A52" t="s">
         <v>19</v>
       </c>
@@ -3343,7 +3492,7 @@
         <v>50000</v>
       </c>
     </row>
-    <row r="53" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A53" t="s">
         <v>20</v>
       </c>
@@ -3354,7 +3503,7 @@
         <v>300000</v>
       </c>
     </row>
-    <row r="54" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A54" t="s">
         <v>21</v>
       </c>
@@ -3365,7 +3514,7 @@
         <v>200000</v>
       </c>
     </row>
-    <row r="55" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A55" t="s">
         <v>22</v>
       </c>
@@ -3376,7 +3525,7 @@
         <v>100000</v>
       </c>
     </row>
-    <row r="56" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A56" t="s">
         <v>37</v>
       </c>
@@ -3387,7 +3536,7 @@
         <v>30000</v>
       </c>
     </row>
-    <row r="57" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A57" t="s">
         <v>23</v>
       </c>
@@ -3398,7 +3547,7 @@
         <v>100000</v>
       </c>
     </row>
-    <row r="58" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A58" t="s">
         <v>25</v>
       </c>
@@ -3409,7 +3558,7 @@
         <v>100000</v>
       </c>
     </row>
-    <row r="59" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A59" t="s">
         <v>26</v>
       </c>
@@ -3420,7 +3569,7 @@
         <v>100000</v>
       </c>
     </row>
-    <row r="60" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A60" t="s">
         <v>27</v>
       </c>
@@ -3431,7 +3580,7 @@
         <v>100000</v>
       </c>
     </row>
-    <row r="61" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A61" t="s">
         <v>28</v>
       </c>
@@ -3442,7 +3591,7 @@
         <v>100000</v>
       </c>
     </row>
-    <row r="62" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A62" t="s">
         <v>29</v>
       </c>
@@ -3453,7 +3602,7 @@
         <v>100000</v>
       </c>
     </row>
-    <row r="63" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A63" t="s">
         <v>30</v>
       </c>
@@ -3464,7 +3613,7 @@
         <v>100000</v>
       </c>
     </row>
-    <row r="64" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A64" t="s">
         <v>31</v>
       </c>
@@ -3475,7 +3624,7 @@
         <v>100000</v>
       </c>
     </row>
-    <row r="66" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A66" t="s">
         <v>36</v>
       </c>
@@ -3486,7 +3635,28 @@
         <v>1570</v>
       </c>
     </row>
+    <row r="70" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="B70" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="71" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="B71" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="74" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="B74" s="9">
+        <v>3151000</v>
+      </c>
+    </row>
+    <row r="75" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="B75" s="9">
+        <v>1830000</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>